<commit_message>
fixed team name mismatchs
</commit_message>
<xml_diff>
--- a/stats_averages.xlsx
+++ b/stats_averages.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="full" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="summary" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="full" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="summary" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -4183,33 +4183,69 @@
       <c r="K2" t="n">
         <v>7.649999999999999</v>
       </c>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
+      <c r="L2" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>3/5</t>
+        </is>
+      </c>
       <c r="N2" t="n">
         <v>25.05</v>
       </c>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr"/>
+      <c r="O2" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>4/5</t>
+        </is>
+      </c>
       <c r="Q2" t="n">
         <v>26.5</v>
       </c>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
+      <c r="R2" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>2/5</t>
+        </is>
+      </c>
       <c r="T2" t="n">
         <v>5.25</v>
       </c>
-      <c r="U2" t="inlineStr"/>
-      <c r="V2" t="inlineStr"/>
+      <c r="U2" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>1/5</t>
+        </is>
+      </c>
       <c r="W2" t="n">
         <v>34.65</v>
       </c>
-      <c r="X2" t="inlineStr"/>
-      <c r="Y2" t="inlineStr"/>
+      <c r="X2" t="n">
+        <v>36.5</v>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>2/5</t>
+        </is>
+      </c>
       <c r="Z2" t="n">
         <v>2.277777777777778</v>
       </c>
-      <c r="AA2" t="inlineStr"/>
-      <c r="AB2" t="inlineStr"/>
+      <c r="AA2" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>1/4</t>
+        </is>
+      </c>
       <c r="AC2" t="n">
         <v>9.699999999999999</v>
       </c>
@@ -4305,33 +4341,69 @@
       <c r="K3" t="n">
         <v>9.449999999999999</v>
       </c>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
+      <c r="L3" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>2/3</t>
+        </is>
+      </c>
       <c r="N3" t="n">
         <v>25.1</v>
       </c>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
+      <c r="O3" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>2/3</t>
+        </is>
+      </c>
       <c r="Q3" t="n">
         <v>22.4</v>
       </c>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
+      <c r="R3" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>1/2</t>
+        </is>
+      </c>
       <c r="T3" t="n">
         <v>6.6</v>
       </c>
-      <c r="U3" t="inlineStr"/>
-      <c r="V3" t="inlineStr"/>
+      <c r="U3" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>1/3</t>
+        </is>
+      </c>
       <c r="W3" t="n">
         <v>35.2</v>
       </c>
-      <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="inlineStr"/>
+      <c r="X3" t="n">
+        <v>34.5</v>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>2/3</t>
+        </is>
+      </c>
       <c r="Z3" t="n">
         <v>3.45</v>
       </c>
-      <c r="AA3" t="inlineStr"/>
-      <c r="AB3" t="inlineStr"/>
+      <c r="AA3" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>1/3</t>
+        </is>
+      </c>
       <c r="AC3" t="n">
         <v>9.1</v>
       </c>
@@ -4427,33 +4499,69 @@
       <c r="K4" t="n">
         <v>7.800000000000001</v>
       </c>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
+      <c r="L4" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>4/5</t>
+        </is>
+      </c>
       <c r="N4" t="n">
         <v>25.9</v>
       </c>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
+      <c r="O4" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>4/5</t>
+        </is>
+      </c>
       <c r="Q4" t="n">
         <v>25.7</v>
       </c>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
+      <c r="R4" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>2/5</t>
+        </is>
+      </c>
       <c r="T4" t="n">
         <v>4.95</v>
       </c>
-      <c r="U4" t="inlineStr"/>
-      <c r="V4" t="inlineStr"/>
+      <c r="U4" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>3/5</t>
+        </is>
+      </c>
       <c r="W4" t="n">
         <v>37.65</v>
       </c>
-      <c r="X4" t="inlineStr"/>
-      <c r="Y4" t="inlineStr"/>
+      <c r="X4" t="n">
+        <v>35.5</v>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>1/5</t>
+        </is>
+      </c>
       <c r="Z4" t="n">
         <v>3.625</v>
       </c>
-      <c r="AA4" t="inlineStr"/>
-      <c r="AB4" t="inlineStr"/>
+      <c r="AA4" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>4/4</t>
+        </is>
+      </c>
       <c r="AC4" t="n">
         <v>9</v>
       </c>
@@ -4549,33 +4657,69 @@
       <c r="K5" t="n">
         <v>9.050000000000001</v>
       </c>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
+      <c r="L5" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>3/5</t>
+        </is>
+      </c>
       <c r="N5" t="n">
         <v>26.15</v>
       </c>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
+      <c r="O5" t="n">
+        <v>26.5</v>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>2/5</t>
+        </is>
+      </c>
       <c r="Q5" t="n">
         <v>21.6</v>
       </c>
-      <c r="R5" t="inlineStr"/>
-      <c r="S5" t="inlineStr"/>
+      <c r="R5" t="n">
+        <v>20.5</v>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>3/5</t>
+        </is>
+      </c>
       <c r="T5" t="n">
         <v>6.222222222222222</v>
       </c>
-      <c r="U5" t="inlineStr"/>
-      <c r="V5" t="inlineStr"/>
+      <c r="U5" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>2/5</t>
+        </is>
+      </c>
       <c r="W5" t="n">
         <v>37.5</v>
       </c>
-      <c r="X5" t="inlineStr"/>
-      <c r="Y5" t="inlineStr"/>
+      <c r="X5" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>0/5</t>
+        </is>
+      </c>
       <c r="Z5" t="n">
         <v>2.905555555555556</v>
       </c>
-      <c r="AA5" t="inlineStr"/>
-      <c r="AB5" t="inlineStr"/>
+      <c r="AA5" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t>2/5</t>
+        </is>
+      </c>
       <c r="AC5" t="n">
         <v>9.800000000000001</v>
       </c>
@@ -4829,33 +4973,69 @@
       <c r="K7" t="n">
         <v>8.949999999999999</v>
       </c>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
+      <c r="L7" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>2/3</t>
+        </is>
+      </c>
       <c r="N7" t="n">
         <v>26.7</v>
       </c>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
+      <c r="O7" t="n">
+        <v>26.5</v>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>1/3</t>
+        </is>
+      </c>
       <c r="Q7" t="n">
         <v>20.1</v>
       </c>
-      <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr"/>
+      <c r="R7" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
       <c r="T7" t="n">
         <v>5.85</v>
       </c>
-      <c r="U7" t="inlineStr"/>
-      <c r="V7" t="inlineStr"/>
+      <c r="U7" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>2/3</t>
+        </is>
+      </c>
       <c r="W7" t="n">
         <v>33.35</v>
       </c>
-      <c r="X7" t="inlineStr"/>
-      <c r="Y7" t="inlineStr"/>
+      <c r="X7" t="n">
+        <v>33.5</v>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>2/3</t>
+        </is>
+      </c>
       <c r="Z7" t="n">
         <v>2.883333333333333</v>
       </c>
-      <c r="AA7" t="inlineStr"/>
-      <c r="AB7" t="inlineStr"/>
+      <c r="AA7" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t>2/3</t>
+        </is>
+      </c>
       <c r="AC7" t="n">
         <v>10.6</v>
       </c>
@@ -4952,32 +5132,56 @@
         <v>8.649999999999999</v>
       </c>
       <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>0/5</t>
+        </is>
+      </c>
       <c r="N8" t="n">
         <v>26.1</v>
       </c>
       <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>0/5</t>
+        </is>
+      </c>
       <c r="Q8" t="n">
         <v>22</v>
       </c>
       <c r="R8" t="inlineStr"/>
-      <c r="S8" t="inlineStr"/>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>0/5</t>
+        </is>
+      </c>
       <c r="T8" t="n">
         <v>5.550000000000001</v>
       </c>
       <c r="U8" t="inlineStr"/>
-      <c r="V8" t="inlineStr"/>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>0/5</t>
+        </is>
+      </c>
       <c r="W8" t="n">
         <v>32.8</v>
       </c>
       <c r="X8" t="inlineStr"/>
-      <c r="Y8" t="inlineStr"/>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>0/5</t>
+        </is>
+      </c>
       <c r="Z8" t="n">
         <v>3.6</v>
       </c>
       <c r="AA8" t="inlineStr"/>
-      <c r="AB8" t="inlineStr"/>
+      <c r="AB8" t="inlineStr">
+        <is>
+          <t>0/5</t>
+        </is>
+      </c>
       <c r="AC8" t="n">
         <v>8.300000000000001</v>
       </c>
@@ -5073,33 +5277,69 @@
       <c r="K9" t="n">
         <v>8.800000000000001</v>
       </c>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
+      <c r="L9" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
       <c r="N9" t="n">
         <v>26.15</v>
       </c>
-      <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
+      <c r="O9" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
       <c r="Q9" t="n">
         <v>19.35</v>
       </c>
-      <c r="R9" t="inlineStr"/>
-      <c r="S9" t="inlineStr"/>
+      <c r="R9" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
       <c r="T9" t="n">
         <v>6</v>
       </c>
-      <c r="U9" t="inlineStr"/>
-      <c r="V9" t="inlineStr"/>
+      <c r="U9" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
       <c r="W9" t="n">
         <v>33.85</v>
       </c>
-      <c r="X9" t="inlineStr"/>
-      <c r="Y9" t="inlineStr"/>
+      <c r="X9" t="n">
+        <v>32.5</v>
+      </c>
+      <c r="Y9" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
       <c r="Z9" t="n">
         <v>4.461111111111111</v>
       </c>
-      <c r="AA9" t="inlineStr"/>
-      <c r="AB9" t="inlineStr"/>
+      <c r="AA9" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="AB9" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
       <c r="AC9" t="n">
         <v>10.6</v>
       </c>
@@ -5185,37 +5425,67 @@
         <v>4.305555555555555</v>
       </c>
       <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>0/3</t>
+        </is>
+      </c>
       <c r="K10" t="n">
         <v>11.15</v>
       </c>
       <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>0/3</t>
+        </is>
+      </c>
       <c r="N10" t="n">
         <v>28.95</v>
       </c>
       <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>0/3</t>
+        </is>
+      </c>
       <c r="Q10" t="n">
         <v>22.4</v>
       </c>
       <c r="R10" t="inlineStr"/>
-      <c r="S10" t="inlineStr"/>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>0/3</t>
+        </is>
+      </c>
       <c r="T10" t="n">
         <v>7.4</v>
       </c>
       <c r="U10" t="inlineStr"/>
-      <c r="V10" t="inlineStr"/>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>0/3</t>
+        </is>
+      </c>
       <c r="W10" t="n">
         <v>35.1</v>
       </c>
-      <c r="X10" t="inlineStr"/>
-      <c r="Y10" t="inlineStr"/>
+      <c r="X10" t="n">
+        <v>33.5</v>
+      </c>
+      <c r="Y10" t="inlineStr">
+        <is>
+          <t>1/3</t>
+        </is>
+      </c>
       <c r="Z10" t="n">
         <v>3.316666666666666</v>
       </c>
       <c r="AA10" t="inlineStr"/>
-      <c r="AB10" t="inlineStr"/>
+      <c r="AB10" t="inlineStr">
+        <is>
+          <t>0/2</t>
+        </is>
+      </c>
       <c r="AC10" t="n">
         <v>8.1</v>
       </c>
@@ -5301,37 +5571,67 @@
         <v>4.127777777777778</v>
       </c>
       <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
       <c r="K11" t="n">
         <v>10.4</v>
       </c>
       <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
       <c r="N11" t="n">
         <v>28.55</v>
       </c>
       <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
       <c r="Q11" t="n">
         <v>22.65</v>
       </c>
       <c r="R11" t="inlineStr"/>
-      <c r="S11" t="inlineStr"/>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
       <c r="T11" t="n">
         <v>7.75</v>
       </c>
       <c r="U11" t="inlineStr"/>
-      <c r="V11" t="inlineStr"/>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
       <c r="W11" t="n">
         <v>37.8</v>
       </c>
-      <c r="X11" t="inlineStr"/>
-      <c r="Y11" t="inlineStr"/>
+      <c r="X11" t="n">
+        <v>36.5</v>
+      </c>
+      <c r="Y11" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
       <c r="Z11" t="n">
         <v>3.622222222222222</v>
       </c>
       <c r="AA11" t="inlineStr"/>
-      <c r="AB11" t="inlineStr"/>
+      <c r="AB11" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
       <c r="AC11" t="n">
         <v>9.9</v>
       </c>
@@ -5405,43 +5705,79 @@
       <c r="E12" t="n">
         <v>11.3</v>
       </c>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
+      <c r="F12" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>2/3</t>
+        </is>
+      </c>
       <c r="H12" t="n">
         <v>3.25</v>
       </c>
       <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>0/2</t>
+        </is>
+      </c>
       <c r="K12" t="n">
         <v>10.2</v>
       </c>
       <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>0/3</t>
+        </is>
+      </c>
       <c r="N12" t="n">
         <v>27</v>
       </c>
       <c r="O12" t="inlineStr"/>
-      <c r="P12" t="inlineStr"/>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>0/3</t>
+        </is>
+      </c>
       <c r="Q12" t="n">
         <v>20.1</v>
       </c>
       <c r="R12" t="inlineStr"/>
-      <c r="S12" t="inlineStr"/>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>0/3</t>
+        </is>
+      </c>
       <c r="T12" t="n">
         <v>6.8</v>
       </c>
       <c r="U12" t="inlineStr"/>
-      <c r="V12" t="inlineStr"/>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>0/3</t>
+        </is>
+      </c>
       <c r="W12" t="n">
         <v>35.4</v>
       </c>
-      <c r="X12" t="inlineStr"/>
-      <c r="Y12" t="inlineStr"/>
+      <c r="X12" t="n">
+        <v>34.5</v>
+      </c>
+      <c r="Y12" t="inlineStr">
+        <is>
+          <t>2/3</t>
+        </is>
+      </c>
       <c r="Z12" t="n">
         <v>3.066666666666666</v>
       </c>
       <c r="AA12" t="inlineStr"/>
-      <c r="AB12" t="inlineStr"/>
+      <c r="AB12" t="inlineStr">
+        <is>
+          <t>0/2</t>
+        </is>
+      </c>
       <c r="AC12" t="n">
         <v>12.7</v>
       </c>
@@ -5515,43 +5851,91 @@
       <c r="E13" t="n">
         <v>8.949999999999999</v>
       </c>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
+      <c r="F13" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>3/5</t>
+        </is>
+      </c>
       <c r="H13" t="n">
         <v>4.5625</v>
       </c>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
+      <c r="I13" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>0/5</t>
+        </is>
+      </c>
       <c r="K13" t="n">
         <v>10.85</v>
       </c>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
+      <c r="L13" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>2/5</t>
+        </is>
+      </c>
       <c r="N13" t="n">
         <v>26.5</v>
       </c>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr"/>
+      <c r="O13" t="n">
+        <v>29.5</v>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>2/5</t>
+        </is>
+      </c>
       <c r="Q13" t="n">
         <v>18.8</v>
       </c>
-      <c r="R13" t="inlineStr"/>
-      <c r="S13" t="inlineStr"/>
+      <c r="R13" t="n">
+        <v>17.5</v>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>2/5</t>
+        </is>
+      </c>
       <c r="T13" t="n">
         <v>6.25</v>
       </c>
-      <c r="U13" t="inlineStr"/>
-      <c r="V13" t="inlineStr"/>
+      <c r="U13" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>2/5</t>
+        </is>
+      </c>
       <c r="W13" t="n">
         <v>36.15</v>
       </c>
-      <c r="X13" t="inlineStr"/>
-      <c r="Y13" t="inlineStr"/>
+      <c r="X13" t="n">
+        <v>32.5</v>
+      </c>
+      <c r="Y13" t="inlineStr">
+        <is>
+          <t>2/5</t>
+        </is>
+      </c>
       <c r="Z13" t="n">
         <v>4.35</v>
       </c>
-      <c r="AA13" t="inlineStr"/>
-      <c r="AB13" t="inlineStr"/>
+      <c r="AA13" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="AB13" t="inlineStr">
+        <is>
+          <t>2/5</t>
+        </is>
+      </c>
       <c r="AC13" t="n">
         <v>9.300000000000001</v>
       </c>
@@ -5625,43 +6009,91 @@
       <c r="E14" t="n">
         <v>8.899999999999999</v>
       </c>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
+      <c r="F14" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>1/5</t>
+        </is>
+      </c>
       <c r="H14" t="n">
         <v>3.2</v>
       </c>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
+      <c r="I14" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>2/5</t>
+        </is>
+      </c>
       <c r="K14" t="n">
         <v>9.649999999999999</v>
       </c>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
+      <c r="L14" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>4/5</t>
+        </is>
+      </c>
       <c r="N14" t="n">
         <v>25.5</v>
       </c>
-      <c r="O14" t="inlineStr"/>
-      <c r="P14" t="inlineStr"/>
+      <c r="O14" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>0/5</t>
+        </is>
+      </c>
       <c r="Q14" t="n">
         <v>20.15</v>
       </c>
-      <c r="R14" t="inlineStr"/>
-      <c r="S14" t="inlineStr"/>
+      <c r="R14" t="n">
+        <v>20.5</v>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>2/5</t>
+        </is>
+      </c>
       <c r="T14" t="n">
         <v>5.9</v>
       </c>
-      <c r="U14" t="inlineStr"/>
-      <c r="V14" t="inlineStr"/>
+      <c r="U14" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="V14" t="inlineStr">
+        <is>
+          <t>2/5</t>
+        </is>
+      </c>
       <c r="W14" t="n">
         <v>39.05</v>
       </c>
-      <c r="X14" t="inlineStr"/>
-      <c r="Y14" t="inlineStr"/>
+      <c r="X14" t="n">
+        <v>38.5</v>
+      </c>
+      <c r="Y14" t="inlineStr">
+        <is>
+          <t>1/5</t>
+        </is>
+      </c>
       <c r="Z14" t="n">
         <v>3.333333333333333</v>
       </c>
-      <c r="AA14" t="inlineStr"/>
-      <c r="AB14" t="inlineStr"/>
+      <c r="AA14" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="AB14" t="inlineStr">
+        <is>
+          <t>1/5</t>
+        </is>
+      </c>
       <c r="AC14" t="n">
         <v>8.199999999999999</v>
       </c>
@@ -5735,43 +6167,91 @@
       <c r="E15" t="n">
         <v>9.300000000000001</v>
       </c>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
+      <c r="F15" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>2/5</t>
+        </is>
+      </c>
       <c r="H15" t="n">
         <v>4.2</v>
       </c>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
+      <c r="I15" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>3/5</t>
+        </is>
+      </c>
       <c r="K15" t="n">
         <v>8.5</v>
       </c>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr"/>
+      <c r="L15" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>0/5</t>
+        </is>
+      </c>
       <c r="N15" t="n">
         <v>25</v>
       </c>
-      <c r="O15" t="inlineStr"/>
-      <c r="P15" t="inlineStr"/>
+      <c r="O15" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>2/5</t>
+        </is>
+      </c>
       <c r="Q15" t="n">
         <v>20.3</v>
       </c>
-      <c r="R15" t="inlineStr"/>
-      <c r="S15" t="inlineStr"/>
+      <c r="R15" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>1/5</t>
+        </is>
+      </c>
       <c r="T15" t="n">
         <v>5.6</v>
       </c>
-      <c r="U15" t="inlineStr"/>
-      <c r="V15" t="inlineStr"/>
+      <c r="U15" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="V15" t="inlineStr">
+        <is>
+          <t>3/5</t>
+        </is>
+      </c>
       <c r="W15" t="n">
         <v>37.1</v>
       </c>
-      <c r="X15" t="inlineStr"/>
-      <c r="Y15" t="inlineStr"/>
+      <c r="X15" t="n">
+        <v>34.5</v>
+      </c>
+      <c r="Y15" t="inlineStr">
+        <is>
+          <t>1/5</t>
+        </is>
+      </c>
       <c r="Z15" t="n">
         <v>2.505555555555556</v>
       </c>
-      <c r="AA15" t="inlineStr"/>
-      <c r="AB15" t="inlineStr"/>
+      <c r="AA15" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="AB15" t="inlineStr">
+        <is>
+          <t>2/5</t>
+        </is>
+      </c>
       <c r="AC15" t="n">
         <v>8.800000000000001</v>
       </c>
@@ -5867,33 +6347,69 @@
       <c r="K16" t="n">
         <v>9.25</v>
       </c>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr"/>
+      <c r="L16" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>3/5</t>
+        </is>
+      </c>
       <c r="N16" t="n">
         <v>26.95</v>
       </c>
-      <c r="O16" t="inlineStr"/>
-      <c r="P16" t="inlineStr"/>
+      <c r="O16" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>1/5</t>
+        </is>
+      </c>
       <c r="Q16" t="n">
         <v>21.45</v>
       </c>
-      <c r="R16" t="inlineStr"/>
-      <c r="S16" t="inlineStr"/>
+      <c r="R16" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>3/5</t>
+        </is>
+      </c>
       <c r="T16" t="n">
         <v>6</v>
       </c>
-      <c r="U16" t="inlineStr"/>
-      <c r="V16" t="inlineStr"/>
+      <c r="U16" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="V16" t="inlineStr">
+        <is>
+          <t>4/5</t>
+        </is>
+      </c>
       <c r="W16" t="n">
         <v>39.15000000000001</v>
       </c>
-      <c r="X16" t="inlineStr"/>
-      <c r="Y16" t="inlineStr"/>
+      <c r="X16" t="n">
+        <v>39.5</v>
+      </c>
+      <c r="Y16" t="inlineStr">
+        <is>
+          <t>1/5</t>
+        </is>
+      </c>
       <c r="Z16" t="n">
         <v>3.5</v>
       </c>
-      <c r="AA16" t="inlineStr"/>
-      <c r="AB16" t="inlineStr"/>
+      <c r="AA16" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="AB16" t="inlineStr">
+        <is>
+          <t>0/5</t>
+        </is>
+      </c>
       <c r="AC16" t="n">
         <v>10.5</v>
       </c>
@@ -5989,33 +6505,69 @@
       <c r="K17" t="n">
         <v>9.399999999999999</v>
       </c>
-      <c r="L17" t="inlineStr"/>
-      <c r="M17" t="inlineStr"/>
+      <c r="L17" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>2/3</t>
+        </is>
+      </c>
       <c r="N17" t="n">
         <v>26.65</v>
       </c>
-      <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr"/>
+      <c r="O17" t="n">
+        <v>26.5</v>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>1/3</t>
+        </is>
+      </c>
       <c r="Q17" t="n">
         <v>19.6</v>
       </c>
-      <c r="R17" t="inlineStr"/>
-      <c r="S17" t="inlineStr"/>
+      <c r="R17" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>1/3</t>
+        </is>
+      </c>
       <c r="T17" t="n">
         <v>6.35</v>
       </c>
-      <c r="U17" t="inlineStr"/>
-      <c r="V17" t="inlineStr"/>
+      <c r="U17" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="V17" t="inlineStr">
+        <is>
+          <t>1/3</t>
+        </is>
+      </c>
       <c r="W17" t="n">
         <v>40.9</v>
       </c>
-      <c r="X17" t="inlineStr"/>
-      <c r="Y17" t="inlineStr"/>
+      <c r="X17" t="n">
+        <v>40.5</v>
+      </c>
+      <c r="Y17" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
       <c r="Z17" t="n">
         <v>3.622222222222222</v>
       </c>
-      <c r="AA17" t="inlineStr"/>
-      <c r="AB17" t="inlineStr"/>
+      <c r="AA17" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="AB17" t="inlineStr">
+        <is>
+          <t>1/3</t>
+        </is>
+      </c>
       <c r="AC17" t="n">
         <v>9.300000000000001</v>
       </c>
@@ -6111,33 +6663,69 @@
       <c r="K18" t="n">
         <v>8.5</v>
       </c>
-      <c r="L18" t="inlineStr"/>
-      <c r="M18" t="inlineStr"/>
+      <c r="L18" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
       <c r="N18" t="n">
         <v>25</v>
       </c>
-      <c r="O18" t="inlineStr"/>
-      <c r="P18" t="inlineStr"/>
+      <c r="O18" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
       <c r="Q18" t="n">
         <v>25.45</v>
       </c>
-      <c r="R18" t="inlineStr"/>
-      <c r="S18" t="inlineStr"/>
+      <c r="R18" t="n">
+        <v>26.5</v>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
       <c r="T18" t="n">
         <v>5.7</v>
       </c>
-      <c r="U18" t="inlineStr"/>
-      <c r="V18" t="inlineStr"/>
+      <c r="U18" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="V18" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
       <c r="W18" t="n">
         <v>37.8</v>
       </c>
-      <c r="X18" t="inlineStr"/>
-      <c r="Y18" t="inlineStr"/>
+      <c r="X18" t="n">
+        <v>38.5</v>
+      </c>
+      <c r="Y18" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
       <c r="Z18" t="n">
         <v>4.772222222222222</v>
       </c>
-      <c r="AA18" t="inlineStr"/>
-      <c r="AB18" t="inlineStr"/>
+      <c r="AA18" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="AB18" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
       <c r="AC18" t="n">
         <v>10.5</v>
       </c>
@@ -6211,43 +6799,89 @@
       <c r="E19" t="n">
         <v>10.15</v>
       </c>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
+      <c r="F19" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>2/5</t>
+        </is>
+      </c>
       <c r="H19" t="n">
         <v>4.95</v>
       </c>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
+      <c r="I19" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>2/5</t>
+        </is>
+      </c>
       <c r="K19" t="n">
         <v>9.199999999999999</v>
       </c>
-      <c r="L19" t="inlineStr"/>
-      <c r="M19" t="inlineStr"/>
+      <c r="L19" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>3/5</t>
+        </is>
+      </c>
       <c r="N19" t="n">
         <v>25.35</v>
       </c>
-      <c r="O19" t="inlineStr"/>
-      <c r="P19" t="inlineStr"/>
+      <c r="O19" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>4/5</t>
+        </is>
+      </c>
       <c r="Q19" t="n">
         <v>24.45</v>
       </c>
-      <c r="R19" t="inlineStr"/>
-      <c r="S19" t="inlineStr"/>
+      <c r="R19" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>3/5</t>
+        </is>
+      </c>
       <c r="T19" t="n">
         <v>6.25</v>
       </c>
       <c r="U19" t="inlineStr"/>
-      <c r="V19" t="inlineStr"/>
+      <c r="V19" t="inlineStr">
+        <is>
+          <t>0/5</t>
+        </is>
+      </c>
       <c r="W19" t="n">
         <v>33.2</v>
       </c>
-      <c r="X19" t="inlineStr"/>
-      <c r="Y19" t="inlineStr"/>
+      <c r="X19" t="n">
+        <v>33.5</v>
+      </c>
+      <c r="Y19" t="inlineStr">
+        <is>
+          <t>1/5</t>
+        </is>
+      </c>
       <c r="Z19" t="n">
         <v>2.933333333333334</v>
       </c>
-      <c r="AA19" t="inlineStr"/>
-      <c r="AB19" t="inlineStr"/>
+      <c r="AA19" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="AB19" t="inlineStr">
+        <is>
+          <t>3/4</t>
+        </is>
+      </c>
       <c r="AC19" t="n">
         <v>9</v>
       </c>
@@ -6343,33 +6977,69 @@
       <c r="K20" t="n">
         <v>8.100000000000001</v>
       </c>
-      <c r="L20" t="inlineStr"/>
-      <c r="M20" t="inlineStr"/>
+      <c r="L20" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>2/4</t>
+        </is>
+      </c>
       <c r="N20" t="n">
         <v>23</v>
       </c>
-      <c r="O20" t="inlineStr"/>
-      <c r="P20" t="inlineStr"/>
+      <c r="O20" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>2/4</t>
+        </is>
+      </c>
       <c r="Q20" t="n">
         <v>23.75</v>
       </c>
-      <c r="R20" t="inlineStr"/>
-      <c r="S20" t="inlineStr"/>
+      <c r="R20" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>2/4</t>
+        </is>
+      </c>
       <c r="T20" t="n">
         <v>5.65</v>
       </c>
-      <c r="U20" t="inlineStr"/>
-      <c r="V20" t="inlineStr"/>
+      <c r="U20" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="V20" t="inlineStr">
+        <is>
+          <t>2/4</t>
+        </is>
+      </c>
       <c r="W20" t="n">
         <v>37.05</v>
       </c>
-      <c r="X20" t="inlineStr"/>
-      <c r="Y20" t="inlineStr"/>
+      <c r="X20" t="n">
+        <v>35.5</v>
+      </c>
+      <c r="Y20" t="inlineStr">
+        <is>
+          <t>1/4</t>
+        </is>
+      </c>
       <c r="Z20" t="n">
         <v>4</v>
       </c>
-      <c r="AA20" t="inlineStr"/>
-      <c r="AB20" t="inlineStr"/>
+      <c r="AA20" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="AB20" t="inlineStr">
+        <is>
+          <t>3/4</t>
+        </is>
+      </c>
       <c r="AC20" t="n">
         <v>10.9</v>
       </c>
@@ -6465,33 +7135,69 @@
       <c r="K21" t="n">
         <v>10.25</v>
       </c>
-      <c r="L21" t="inlineStr"/>
-      <c r="M21" t="inlineStr"/>
+      <c r="L21" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>2/5</t>
+        </is>
+      </c>
       <c r="N21" t="n">
         <v>28.15</v>
       </c>
-      <c r="O21" t="inlineStr"/>
-      <c r="P21" t="inlineStr"/>
+      <c r="O21" t="n">
+        <v>26.5</v>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>3/5</t>
+        </is>
+      </c>
       <c r="Q21" t="n">
         <v>24.2</v>
       </c>
-      <c r="R21" t="inlineStr"/>
-      <c r="S21" t="inlineStr"/>
+      <c r="R21" t="n">
+        <v>26.5</v>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>3/5</t>
+        </is>
+      </c>
       <c r="T21" t="n">
         <v>7.25</v>
       </c>
-      <c r="U21" t="inlineStr"/>
-      <c r="V21" t="inlineStr"/>
+      <c r="U21" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="V21" t="inlineStr">
+        <is>
+          <t>3/5</t>
+        </is>
+      </c>
       <c r="W21" t="n">
         <v>39.55</v>
       </c>
-      <c r="X21" t="inlineStr"/>
-      <c r="Y21" t="inlineStr"/>
+      <c r="X21" t="n">
+        <v>35.5</v>
+      </c>
+      <c r="Y21" t="inlineStr">
+        <is>
+          <t>4/5</t>
+        </is>
+      </c>
       <c r="Z21" t="n">
         <v>4.1</v>
       </c>
-      <c r="AA21" t="inlineStr"/>
-      <c r="AB21" t="inlineStr"/>
+      <c r="AA21" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="AB21" t="inlineStr">
+        <is>
+          <t>3/5</t>
+        </is>
+      </c>
       <c r="AC21" t="n">
         <v>10</v>
       </c>
@@ -6576,38 +7282,70 @@
       <c r="H22" t="n">
         <v>4.394444444444445</v>
       </c>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr"/>
+      <c r="I22" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
       <c r="K22" t="n">
         <v>9.5</v>
       </c>
       <c r="L22" t="inlineStr"/>
-      <c r="M22" t="inlineStr"/>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
       <c r="N22" t="n">
         <v>27.2</v>
       </c>
       <c r="O22" t="inlineStr"/>
-      <c r="P22" t="inlineStr"/>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
       <c r="Q22" t="n">
         <v>26.35</v>
       </c>
       <c r="R22" t="inlineStr"/>
-      <c r="S22" t="inlineStr"/>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
       <c r="T22" t="n">
         <v>5.949999999999999</v>
       </c>
       <c r="U22" t="inlineStr"/>
-      <c r="V22" t="inlineStr"/>
+      <c r="V22" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
       <c r="W22" t="n">
         <v>40.3</v>
       </c>
-      <c r="X22" t="inlineStr"/>
-      <c r="Y22" t="inlineStr"/>
+      <c r="X22" t="n">
+        <v>41.5</v>
+      </c>
+      <c r="Y22" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
       <c r="Z22" t="n">
         <v>4.2</v>
       </c>
       <c r="AA22" t="inlineStr"/>
-      <c r="AB22" t="inlineStr"/>
+      <c r="AB22" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
       <c r="AC22" t="n">
         <v>9.199999999999999</v>
       </c>
@@ -6692,38 +7430,70 @@
       <c r="H23" t="n">
         <v>4.372222222222222</v>
       </c>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
+      <c r="I23" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>0/3</t>
+        </is>
+      </c>
       <c r="K23" t="n">
         <v>9.35</v>
       </c>
       <c r="L23" t="inlineStr"/>
-      <c r="M23" t="inlineStr"/>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>0/3</t>
+        </is>
+      </c>
       <c r="N23" t="n">
         <v>25.2</v>
       </c>
       <c r="O23" t="inlineStr"/>
-      <c r="P23" t="inlineStr"/>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>0/3</t>
+        </is>
+      </c>
       <c r="Q23" t="n">
         <v>26.6</v>
       </c>
       <c r="R23" t="inlineStr"/>
-      <c r="S23" t="inlineStr"/>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>0/3</t>
+        </is>
+      </c>
       <c r="T23" t="n">
         <v>6.25</v>
       </c>
       <c r="U23" t="inlineStr"/>
-      <c r="V23" t="inlineStr"/>
+      <c r="V23" t="inlineStr">
+        <is>
+          <t>0/3</t>
+        </is>
+      </c>
       <c r="W23" t="n">
         <v>34.35</v>
       </c>
-      <c r="X23" t="inlineStr"/>
-      <c r="Y23" t="inlineStr"/>
+      <c r="X23" t="n">
+        <v>35.5</v>
+      </c>
+      <c r="Y23" t="inlineStr">
+        <is>
+          <t>1/3</t>
+        </is>
+      </c>
       <c r="Z23" t="n">
         <v>3.5</v>
       </c>
       <c r="AA23" t="inlineStr"/>
-      <c r="AB23" t="inlineStr"/>
+      <c r="AB23" t="inlineStr">
+        <is>
+          <t>0/3</t>
+        </is>
+      </c>
       <c r="AC23" t="n">
         <v>8.9</v>
       </c>
@@ -6808,38 +7578,70 @@
       <c r="H24" t="n">
         <v>4.65</v>
       </c>
-      <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr"/>
+      <c r="I24" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>0/3</t>
+        </is>
+      </c>
       <c r="K24" t="n">
         <v>8.5</v>
       </c>
       <c r="L24" t="inlineStr"/>
-      <c r="M24" t="inlineStr"/>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>0/3</t>
+        </is>
+      </c>
       <c r="N24" t="n">
         <v>27.4</v>
       </c>
       <c r="O24" t="inlineStr"/>
-      <c r="P24" t="inlineStr"/>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>0/3</t>
+        </is>
+      </c>
       <c r="Q24" t="n">
         <v>24.25</v>
       </c>
       <c r="R24" t="inlineStr"/>
-      <c r="S24" t="inlineStr"/>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>0/3</t>
+        </is>
+      </c>
       <c r="T24" t="n">
         <v>5.4</v>
       </c>
       <c r="U24" t="inlineStr"/>
-      <c r="V24" t="inlineStr"/>
+      <c r="V24" t="inlineStr">
+        <is>
+          <t>0/3</t>
+        </is>
+      </c>
       <c r="W24" t="n">
         <v>36.9</v>
       </c>
-      <c r="X24" t="inlineStr"/>
-      <c r="Y24" t="inlineStr"/>
+      <c r="X24" t="n">
+        <v>36.5</v>
+      </c>
+      <c r="Y24" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
       <c r="Z24" t="n">
         <v>3.5</v>
       </c>
       <c r="AA24" t="inlineStr"/>
-      <c r="AB24" t="inlineStr"/>
+      <c r="AB24" t="inlineStr">
+        <is>
+          <t>0/3</t>
+        </is>
+      </c>
       <c r="AC24" t="n">
         <v>8.199999999999999</v>
       </c>
@@ -6913,43 +7715,87 @@
       <c r="E25" t="n">
         <v>8.550000000000001</v>
       </c>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
+      <c r="F25" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>2/3</t>
+        </is>
+      </c>
       <c r="H25" t="n">
         <v>3.111111111111111</v>
       </c>
-      <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr"/>
+      <c r="I25" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
       <c r="K25" t="n">
         <v>9.800000000000001</v>
       </c>
-      <c r="L25" t="inlineStr"/>
-      <c r="M25" t="inlineStr"/>
+      <c r="L25" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
       <c r="N25" t="n">
         <v>25.85</v>
       </c>
-      <c r="O25" t="inlineStr"/>
-      <c r="P25" t="inlineStr"/>
+      <c r="O25" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
       <c r="Q25" t="n">
         <v>19.6</v>
       </c>
-      <c r="R25" t="inlineStr"/>
-      <c r="S25" t="inlineStr"/>
+      <c r="R25" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
       <c r="T25" t="n">
         <v>6.8</v>
       </c>
       <c r="U25" t="inlineStr"/>
-      <c r="V25" t="inlineStr"/>
+      <c r="V25" t="inlineStr">
+        <is>
+          <t>0/3</t>
+        </is>
+      </c>
       <c r="W25" t="n">
         <v>32.45</v>
       </c>
       <c r="X25" t="inlineStr"/>
-      <c r="Y25" t="inlineStr"/>
+      <c r="Y25" t="inlineStr">
+        <is>
+          <t>0/3</t>
+        </is>
+      </c>
       <c r="Z25" t="n">
         <v>3.708333333333333</v>
       </c>
-      <c r="AA25" t="inlineStr"/>
-      <c r="AB25" t="inlineStr"/>
+      <c r="AA25" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AB25" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
       <c r="AC25" t="n">
         <v>9.4</v>
       </c>
@@ -7045,33 +7891,69 @@
       <c r="K26" t="n">
         <v>7.8</v>
       </c>
-      <c r="L26" t="inlineStr"/>
-      <c r="M26" t="inlineStr"/>
+      <c r="L26" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
       <c r="N26" t="n">
         <v>22.75</v>
       </c>
-      <c r="O26" t="inlineStr"/>
-      <c r="P26" t="inlineStr"/>
+      <c r="O26" t="n">
+        <v>23.5</v>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
       <c r="Q26" t="n">
         <v>25.2</v>
       </c>
-      <c r="R26" t="inlineStr"/>
-      <c r="S26" t="inlineStr"/>
+      <c r="R26" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
       <c r="T26" t="n">
         <v>5.3</v>
       </c>
-      <c r="U26" t="inlineStr"/>
-      <c r="V26" t="inlineStr"/>
+      <c r="U26" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="V26" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
       <c r="W26" t="n">
         <v>34.25</v>
       </c>
-      <c r="X26" t="inlineStr"/>
-      <c r="Y26" t="inlineStr"/>
+      <c r="X26" t="n">
+        <v>35.5</v>
+      </c>
+      <c r="Y26" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
       <c r="Z26" t="n">
         <v>3.222222222222222</v>
       </c>
-      <c r="AA26" t="inlineStr"/>
-      <c r="AB26" t="inlineStr"/>
+      <c r="AA26" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="AB26" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
       <c r="AC26" t="n">
         <v>9.199999999999999</v>
       </c>
@@ -7167,33 +8049,69 @@
       <c r="K27" t="n">
         <v>8.550000000000001</v>
       </c>
-      <c r="L27" t="inlineStr"/>
-      <c r="M27" t="inlineStr"/>
+      <c r="L27" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>4/5</t>
+        </is>
+      </c>
       <c r="N27" t="n">
         <v>24.3</v>
       </c>
-      <c r="O27" t="inlineStr"/>
-      <c r="P27" t="inlineStr"/>
+      <c r="O27" t="n">
+        <v>26.5</v>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>2/5</t>
+        </is>
+      </c>
       <c r="Q27" t="n">
         <v>26.15</v>
       </c>
-      <c r="R27" t="inlineStr"/>
-      <c r="S27" t="inlineStr"/>
+      <c r="R27" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>2/5</t>
+        </is>
+      </c>
       <c r="T27" t="n">
         <v>6.05</v>
       </c>
-      <c r="U27" t="inlineStr"/>
-      <c r="V27" t="inlineStr"/>
+      <c r="U27" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="V27" t="inlineStr">
+        <is>
+          <t>2/5</t>
+        </is>
+      </c>
       <c r="W27" t="n">
         <v>38.35</v>
       </c>
-      <c r="X27" t="inlineStr"/>
-      <c r="Y27" t="inlineStr"/>
+      <c r="X27" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="Y27" t="inlineStr">
+        <is>
+          <t>1/5</t>
+        </is>
+      </c>
       <c r="Z27" t="n">
         <v>4.284722222222222</v>
       </c>
-      <c r="AA27" t="inlineStr"/>
-      <c r="AB27" t="inlineStr"/>
+      <c r="AA27" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="AB27" t="inlineStr">
+        <is>
+          <t>3/4</t>
+        </is>
+      </c>
       <c r="AC27" t="n">
         <v>7.7</v>
       </c>
@@ -7278,38 +8196,70 @@
       <c r="H28" t="n">
         <v>5.35</v>
       </c>
-      <c r="I28" t="inlineStr"/>
-      <c r="J28" t="inlineStr"/>
+      <c r="I28" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
       <c r="K28" t="n">
         <v>7.1</v>
       </c>
       <c r="L28" t="inlineStr"/>
-      <c r="M28" t="inlineStr"/>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
       <c r="N28" t="n">
         <v>22.15</v>
       </c>
       <c r="O28" t="inlineStr"/>
-      <c r="P28" t="inlineStr"/>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
       <c r="Q28" t="n">
         <v>28.4</v>
       </c>
       <c r="R28" t="inlineStr"/>
-      <c r="S28" t="inlineStr"/>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
       <c r="T28" t="n">
         <v>5.077777777777778</v>
       </c>
       <c r="U28" t="inlineStr"/>
-      <c r="V28" t="inlineStr"/>
+      <c r="V28" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
       <c r="W28" t="n">
         <v>40</v>
       </c>
-      <c r="X28" t="inlineStr"/>
-      <c r="Y28" t="inlineStr"/>
+      <c r="X28" t="n">
+        <v>40.5</v>
+      </c>
+      <c r="Y28" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
       <c r="Z28" t="n">
         <v>2.761111111111111</v>
       </c>
       <c r="AA28" t="inlineStr"/>
-      <c r="AB28" t="inlineStr"/>
+      <c r="AB28" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
       <c r="AC28" t="n">
         <v>8.699999999999999</v>
       </c>
@@ -7394,38 +8344,70 @@
       <c r="H29" t="n">
         <v>5.45</v>
       </c>
-      <c r="I29" t="inlineStr"/>
-      <c r="J29" t="inlineStr"/>
+      <c r="I29" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
       <c r="K29" t="n">
         <v>8.5</v>
       </c>
       <c r="L29" t="inlineStr"/>
-      <c r="M29" t="inlineStr"/>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>0/3</t>
+        </is>
+      </c>
       <c r="N29" t="n">
         <v>25.5</v>
       </c>
       <c r="O29" t="inlineStr"/>
-      <c r="P29" t="inlineStr"/>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>0/3</t>
+        </is>
+      </c>
       <c r="Q29" t="n">
         <v>26</v>
       </c>
       <c r="R29" t="inlineStr"/>
-      <c r="S29" t="inlineStr"/>
+      <c r="S29" t="inlineStr">
+        <is>
+          <t>0/3</t>
+        </is>
+      </c>
       <c r="T29" t="n">
         <v>5.45</v>
       </c>
       <c r="U29" t="inlineStr"/>
-      <c r="V29" t="inlineStr"/>
+      <c r="V29" t="inlineStr">
+        <is>
+          <t>0/3</t>
+        </is>
+      </c>
       <c r="W29" t="n">
         <v>40.59999999999999</v>
       </c>
-      <c r="X29" t="inlineStr"/>
-      <c r="Y29" t="inlineStr"/>
+      <c r="X29" t="n">
+        <v>43.5</v>
+      </c>
+      <c r="Y29" t="inlineStr">
+        <is>
+          <t>1/3</t>
+        </is>
+      </c>
       <c r="Z29" t="n">
         <v>4.4</v>
       </c>
       <c r="AA29" t="inlineStr"/>
-      <c r="AB29" t="inlineStr"/>
+      <c r="AB29" t="inlineStr">
+        <is>
+          <t>0/3</t>
+        </is>
+      </c>
       <c r="AC29" t="n">
         <v>8.800000000000001</v>
       </c>
@@ -7510,8 +8492,14 @@
       <c r="H30" t="n">
         <v>5.15</v>
       </c>
-      <c r="I30" t="inlineStr"/>
-      <c r="J30" t="inlineStr"/>
+      <c r="I30" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>2/5</t>
+        </is>
+      </c>
       <c r="K30" t="n">
         <v>8.199999999999999</v>
       </c>
@@ -7549,17 +8537,31 @@
         <v>5.7</v>
       </c>
       <c r="U30" t="inlineStr"/>
-      <c r="V30" t="inlineStr"/>
+      <c r="V30" t="inlineStr">
+        <is>
+          <t>0/5</t>
+        </is>
+      </c>
       <c r="W30" t="n">
         <v>34.90000000000001</v>
       </c>
-      <c r="X30" t="inlineStr"/>
-      <c r="Y30" t="inlineStr"/>
+      <c r="X30" t="n">
+        <v>33.5</v>
+      </c>
+      <c r="Y30" t="inlineStr">
+        <is>
+          <t>3/5</t>
+        </is>
+      </c>
       <c r="Z30" t="n">
         <v>3.444444444444445</v>
       </c>
       <c r="AA30" t="inlineStr"/>
-      <c r="AB30" t="inlineStr"/>
+      <c r="AB30" t="inlineStr">
+        <is>
+          <t>0/4</t>
+        </is>
+      </c>
       <c r="AC30" t="n">
         <v>7.7</v>
       </c>
@@ -7633,43 +8635,81 @@
       <c r="E31" t="n">
         <v>8.550000000000001</v>
       </c>
-      <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
+      <c r="F31" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>1/5</t>
+        </is>
+      </c>
       <c r="H31" t="n">
         <v>5.4</v>
       </c>
-      <c r="I31" t="inlineStr"/>
-      <c r="J31" t="inlineStr"/>
+      <c r="I31" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>4/5</t>
+        </is>
+      </c>
       <c r="K31" t="n">
         <v>8.199999999999999</v>
       </c>
       <c r="L31" t="inlineStr"/>
-      <c r="M31" t="inlineStr"/>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>0/5</t>
+        </is>
+      </c>
       <c r="N31" t="n">
         <v>23.15</v>
       </c>
       <c r="O31" t="inlineStr"/>
-      <c r="P31" t="inlineStr"/>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>0/5</t>
+        </is>
+      </c>
       <c r="Q31" t="n">
         <v>27.75</v>
       </c>
       <c r="R31" t="inlineStr"/>
-      <c r="S31" t="inlineStr"/>
+      <c r="S31" t="inlineStr">
+        <is>
+          <t>0/5</t>
+        </is>
+      </c>
       <c r="T31" t="n">
         <v>5.35</v>
       </c>
       <c r="U31" t="inlineStr"/>
-      <c r="V31" t="inlineStr"/>
+      <c r="V31" t="inlineStr">
+        <is>
+          <t>0/5</t>
+        </is>
+      </c>
       <c r="W31" t="n">
         <v>37.75</v>
       </c>
-      <c r="X31" t="inlineStr"/>
-      <c r="Y31" t="inlineStr"/>
+      <c r="X31" t="n">
+        <v>40.5</v>
+      </c>
+      <c r="Y31" t="inlineStr">
+        <is>
+          <t>3/5</t>
+        </is>
+      </c>
       <c r="Z31" t="n">
         <v>2.805555555555555</v>
       </c>
       <c r="AA31" t="inlineStr"/>
-      <c r="AB31" t="inlineStr"/>
+      <c r="AB31" t="inlineStr">
+        <is>
+          <t>0/4</t>
+        </is>
+      </c>
       <c r="AC31" t="n">
         <v>8.9</v>
       </c>
@@ -7743,43 +8783,81 @@
       <c r="E32" t="n">
         <v>9.300000000000001</v>
       </c>
-      <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr"/>
+      <c r="F32" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>1/2</t>
+        </is>
+      </c>
       <c r="H32" t="n">
         <v>5.25</v>
       </c>
-      <c r="I32" t="inlineStr"/>
-      <c r="J32" t="inlineStr"/>
+      <c r="I32" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>0/2</t>
+        </is>
+      </c>
       <c r="K32" t="n">
         <v>8.75</v>
       </c>
       <c r="L32" t="inlineStr"/>
-      <c r="M32" t="inlineStr"/>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>0/2</t>
+        </is>
+      </c>
       <c r="N32" t="n">
         <v>25.25</v>
       </c>
       <c r="O32" t="inlineStr"/>
-      <c r="P32" t="inlineStr"/>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>0/2</t>
+        </is>
+      </c>
       <c r="Q32" t="n">
         <v>25.5</v>
       </c>
       <c r="R32" t="inlineStr"/>
-      <c r="S32" t="inlineStr"/>
+      <c r="S32" t="inlineStr">
+        <is>
+          <t>0/2</t>
+        </is>
+      </c>
       <c r="T32" t="n">
         <v>5.699999999999999</v>
       </c>
       <c r="U32" t="inlineStr"/>
-      <c r="V32" t="inlineStr"/>
+      <c r="V32" t="inlineStr">
+        <is>
+          <t>0/2</t>
+        </is>
+      </c>
       <c r="W32" t="n">
         <v>39.9</v>
       </c>
-      <c r="X32" t="inlineStr"/>
-      <c r="Y32" t="inlineStr"/>
+      <c r="X32" t="n">
+        <v>38.5</v>
+      </c>
+      <c r="Y32" t="inlineStr">
+        <is>
+          <t>0/2</t>
+        </is>
+      </c>
       <c r="Z32" t="n">
         <v>3.038888888888889</v>
       </c>
       <c r="AA32" t="inlineStr"/>
-      <c r="AB32" t="inlineStr"/>
+      <c r="AB32" t="inlineStr">
+        <is>
+          <t>0/2</t>
+        </is>
+      </c>
       <c r="AC32" t="n">
         <v>8.9</v>
       </c>

</xml_diff>